<commit_message>
250915 v. 0.1 Segundo avance
</commit_message>
<xml_diff>
--- a/data/afiliaciones/15_Mexico.xlsx
+++ b/data/afiliaciones/15_Mexico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Salamandra/afiliacion/data/afiliaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6FACE2-1C75-B64D-985F-6BEE7112E9F1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142F25C6-29C1-0949-9A3C-090C7777C165}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="4320" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="15_Mexico" sheetId="1" r:id="rId1"/>
@@ -1190,10 +1190,16 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>